<commit_message>
Utilitaire USB + alerte autocardio + seuils from SD
</commit_message>
<xml_diff>
--- a/schemas/PCB/BOM-BODYGUARD.xlsx
+++ b/schemas/PCB/BOM-BODYGUARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Van_Straat\Desktop\Orange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Van_Straat\Documents\GitHub\braceletquentin\schemas\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>MOUNTING TECHNOLOGY</t>
   </si>
@@ -265,6 +265,30 @@
   </si>
   <si>
     <t>Q1</t>
+  </si>
+  <si>
+    <t>Potentimètre variable 100KOhms</t>
+  </si>
+  <si>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>TC33X-2-104E</t>
+  </si>
+  <si>
+    <t>VR1</t>
+  </si>
+  <si>
+    <t>Ampli audio</t>
+  </si>
+  <si>
+    <t>MAX4466EXK+T</t>
+  </si>
+  <si>
+    <t>MAXIMUM INTEGRATED PRODUCTS</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
 </sst>
 </file>
@@ -275,7 +299,7 @@
     <numFmt numFmtId="164" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -327,6 +351,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -407,6 +438,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -817,10 +849,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1331,6 +1363,58 @@
         <v>80</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1689864</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="15">
+        <v>2514501</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.62992125984251968" header="0.23622047244094491" footer="0.51181102362204722"/>

</xml_diff>